<commit_message>
further optimization, about 2x as fast
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -22,6 +22,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ml-100k_all_included'!$M$1:$M$181</definedName>
+    <definedName name="ml_100k_all_included" localSheetId="2">'raw_ml-100k_all_included'!$M$1:$W$181</definedName>
+    <definedName name="ml_100k_all_included_2" localSheetId="2">'raw_ml-100k_all_included'!$M$1:$W$181</definedName>
     <definedName name="ml_100k_matched_only" localSheetId="4">'raw (e2)'!$A$1:$K$181</definedName>
     <definedName name="ml_1m_all_included" localSheetId="6">'raw_ml-1m_all_included'!$A$1:$K$181</definedName>
     <definedName name="results" localSheetId="3">'matched only (e2)'!$B$2:$L$181</definedName>
@@ -30,7 +32,7 @@
     <definedName name="results.1" localSheetId="3">'matched only (e2)'!$B$2:$L$181</definedName>
     <definedName name="results.1" localSheetId="0">'ml-100k_all_included'!$B$2:$L$181</definedName>
     <definedName name="results.1" localSheetId="5">'ml-1m_all_included'!$B$2:$L$181</definedName>
-    <definedName name="results.1" localSheetId="2">'raw_ml-100k_all_included'!$A$1:$K$180</definedName>
+    <definedName name="results.1" localSheetId="2">'raw_ml-100k_all_included'!$A$2:$K$181</definedName>
     <definedName name="results2_1" localSheetId="3">'matched only (e2)'!$B$2:$L$181</definedName>
     <definedName name="results2_1" localSheetId="5">'ml-1m_all_included'!$B$2:$L$181</definedName>
   </definedNames>
@@ -48,7 +50,41 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ml-100k_matched_only" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="ml-100k_all_included" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/ml-100k_all_included.txt" space="1" consecutive="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="ml-100k_all_included11" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/ml-100k_all_included.txt" space="1" consecutive="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="ml-100k_matched_only" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/ml-100k_matched_only.txt" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -65,7 +101,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="ml-1m_all_included" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="ml-1m_all_included" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/ml-1m_all_included.txt" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -82,7 +118,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="results.1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="results.1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.1.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -99,7 +135,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="results.11" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="results.11" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.1.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -116,7 +152,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="results.111" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="results.111" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.1.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -133,7 +169,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="results.1111" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="results.1111" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.1.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -150,7 +186,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="results1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="results1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -167,7 +203,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="results11" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="results11" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -184,7 +220,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="results111" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="results111" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results.txt" tab="0" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -201,7 +237,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="results21" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="12" name="results21" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results2.txt" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -218,7 +254,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="results211" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="results211" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" codePage="10000" sourceFile="/Users/tyler/Developer/MachineLearning/moivelens/moivelens/results2.txt" space="1" consecutive="1">
       <textFields count="11">
         <textField/>
@@ -239,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="34">
   <si>
     <t>k</t>
   </si>
@@ -1812,47 +1848,55 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results2_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-1m_all_included" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results2_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-1m_all_included" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-100k_all_included_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results2_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-100k_all_included" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results2_1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-100k_matched_only" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results.1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ml-100k_matched_only" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13006,10 +13050,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13022,42 +13066,52 @@
     <col min="7" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1682</v>
-      </c>
-      <c r="D1">
-        <v>1000</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1">
-        <v>0.72592599999999996</v>
-      </c>
-      <c r="H1">
-        <v>1.0212699999999999</v>
-      </c>
-      <c r="I1">
-        <v>0.85535000000000005</v>
-      </c>
-      <c r="J1">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="K1">
-        <v>0</v>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -13089,7 +13143,7 @@
         <v>0.85535000000000005</v>
       </c>
       <c r="J2">
-        <v>0.36599999999999999</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -13124,7 +13178,7 @@
         <v>0.85535000000000005</v>
       </c>
       <c r="J3">
-        <v>0.35299999999999998</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -13132,7 +13186,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -13150,16 +13204,16 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>0.76873999999999998</v>
+        <v>0.72592599999999996</v>
       </c>
       <c r="H4">
-        <v>1.0281199999999999</v>
+        <v>1.0212699999999999</v>
       </c>
       <c r="I4">
-        <v>0.92610000000000003</v>
+        <v>0.85535000000000005</v>
       </c>
       <c r="J4">
-        <v>0.38</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -13194,7 +13248,7 @@
         <v>0.92610000000000003</v>
       </c>
       <c r="J5">
-        <v>0.40300000000000002</v>
+        <v>0.38</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -13229,7 +13283,7 @@
         <v>0.92610000000000003</v>
       </c>
       <c r="J6">
-        <v>0.39800000000000002</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -13237,7 +13291,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -13255,16 +13309,16 @@
         <v>11</v>
       </c>
       <c r="G7">
-        <v>0.77804399999999996</v>
+        <v>0.76873999999999998</v>
       </c>
       <c r="H7">
-        <v>1.01464</v>
+        <v>1.0281199999999999</v>
       </c>
       <c r="I7">
-        <v>0.95914999999999995</v>
+        <v>0.92610000000000003</v>
       </c>
       <c r="J7">
-        <v>0.42499999999999999</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -13299,7 +13353,7 @@
         <v>0.95914999999999995</v>
       </c>
       <c r="J8">
-        <v>0.41499999999999998</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -13334,7 +13388,7 @@
         <v>0.95914999999999995</v>
       </c>
       <c r="J9">
-        <v>0.48399999999999999</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -13342,10 +13396,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1682</v>
@@ -13360,16 +13414,16 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>0.201156</v>
+        <v>0.77804399999999996</v>
       </c>
       <c r="H10">
-        <v>0.59156699999999995</v>
+        <v>1.01464</v>
       </c>
       <c r="I10">
-        <v>0.20974999999999999</v>
+        <v>0.95914999999999995</v>
       </c>
       <c r="J10">
-        <v>0.34399999999999997</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -13404,7 +13458,7 @@
         <v>0.20974999999999999</v>
       </c>
       <c r="J11">
-        <v>0.32600000000000001</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -13439,7 +13493,7 @@
         <v>0.20974999999999999</v>
       </c>
       <c r="J12">
-        <v>0.34</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -13447,7 +13501,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -13465,16 +13519,16 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <v>0.28686200000000001</v>
+        <v>0.201156</v>
       </c>
       <c r="H13">
-        <v>0.69525099999999995</v>
+        <v>0.59156699999999995</v>
       </c>
       <c r="I13">
-        <v>0.30345</v>
+        <v>0.20974999999999999</v>
       </c>
       <c r="J13">
-        <v>0.34100000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -13509,7 +13563,7 @@
         <v>0.30345</v>
       </c>
       <c r="J14">
-        <v>0.32500000000000001</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -13544,7 +13598,7 @@
         <v>0.30345</v>
       </c>
       <c r="J15">
-        <v>0.34499999999999997</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -13552,7 +13606,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -13570,16 +13624,16 @@
         <v>11</v>
       </c>
       <c r="G16">
-        <v>0.38518999999999998</v>
+        <v>0.28686200000000001</v>
       </c>
       <c r="H16">
-        <v>0.79333799999999999</v>
+        <v>0.69525099999999995</v>
       </c>
       <c r="I16">
-        <v>0.41284999999999999</v>
+        <v>0.30345</v>
       </c>
       <c r="J16">
-        <v>0.33800000000000002</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -13614,7 +13668,7 @@
         <v>0.41284999999999999</v>
       </c>
       <c r="J17">
-        <v>0.35299999999999998</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -13649,7 +13703,7 @@
         <v>0.41284999999999999</v>
       </c>
       <c r="J18">
-        <v>0.34399999999999997</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -13657,10 +13711,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>1682</v>
@@ -13675,16 +13729,16 @@
         <v>11</v>
       </c>
       <c r="G19">
-        <v>0.26078099999999999</v>
+        <v>0.38518999999999998</v>
       </c>
       <c r="H19">
-        <v>0.67881899999999995</v>
+        <v>0.79333799999999999</v>
       </c>
       <c r="I19">
-        <v>0.24840000000000001</v>
+        <v>0.41284999999999999</v>
       </c>
       <c r="J19">
-        <v>0.34</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -13719,7 +13773,7 @@
         <v>0.24840000000000001</v>
       </c>
       <c r="J20">
-        <v>0.35699999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -13754,7 +13808,7 @@
         <v>0.24840000000000001</v>
       </c>
       <c r="J21">
-        <v>0.36499999999999999</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -13762,7 +13816,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -13780,13 +13834,13 @@
         <v>11</v>
       </c>
       <c r="G22">
-        <v>0.342198</v>
+        <v>0.26078099999999999</v>
       </c>
       <c r="H22">
-        <v>0.76550200000000002</v>
+        <v>0.67881899999999995</v>
       </c>
       <c r="I22">
-        <v>0.33794999999999997</v>
+        <v>0.24840000000000001</v>
       </c>
       <c r="J22">
         <v>0.36499999999999999</v>
@@ -13824,7 +13878,7 @@
         <v>0.33794999999999997</v>
       </c>
       <c r="J23">
-        <v>0.35499999999999998</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -13859,7 +13913,7 @@
         <v>0.33794999999999997</v>
       </c>
       <c r="J24">
-        <v>0.33200000000000002</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -13867,7 +13921,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -13885,16 +13939,16 @@
         <v>11</v>
       </c>
       <c r="G25">
-        <v>0.43871900000000003</v>
+        <v>0.342198</v>
       </c>
       <c r="H25">
-        <v>0.84711700000000001</v>
+        <v>0.76550200000000002</v>
       </c>
       <c r="I25">
-        <v>0.44969999999999999</v>
+        <v>0.33794999999999997</v>
       </c>
       <c r="J25">
-        <v>0.35099999999999998</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -13929,7 +13983,7 @@
         <v>0.44969999999999999</v>
       </c>
       <c r="J26">
-        <v>0.35599999999999998</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -13964,7 +14018,7 @@
         <v>0.44969999999999999</v>
       </c>
       <c r="J27">
-        <v>0.34599999999999997</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -13972,10 +14026,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>1682</v>
@@ -13990,16 +14044,16 @@
         <v>11</v>
       </c>
       <c r="G28">
-        <v>0.70955800000000002</v>
+        <v>0.43871900000000003</v>
       </c>
       <c r="H28">
-        <v>1.02098</v>
+        <v>0.84711700000000001</v>
       </c>
       <c r="I28">
-        <v>0.82404999999999995</v>
+        <v>0.44969999999999999</v>
       </c>
       <c r="J28">
-        <v>0.38800000000000001</v>
+        <v>0.34599999999999997</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -14034,7 +14088,7 @@
         <v>0.82404999999999995</v>
       </c>
       <c r="J29">
-        <v>0.35499999999999998</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -14077,7 +14131,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -14095,16 +14149,16 @@
         <v>11</v>
       </c>
       <c r="G31">
-        <v>0.75022</v>
+        <v>0.70955800000000002</v>
       </c>
       <c r="H31">
-        <v>1.0186200000000001</v>
+        <v>1.02098</v>
       </c>
       <c r="I31">
-        <v>0.90344999999999998</v>
+        <v>0.82404999999999995</v>
       </c>
       <c r="J31">
-        <v>0.437</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -14139,7 +14193,7 @@
         <v>0.90344999999999998</v>
       </c>
       <c r="J32">
-        <v>0.42799999999999999</v>
+        <v>0.437</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -14174,7 +14228,7 @@
         <v>0.90344999999999998</v>
       </c>
       <c r="J33">
-        <v>0.44600000000000001</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -14182,7 +14236,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -14200,16 +14254,16 @@
         <v>11</v>
       </c>
       <c r="G34">
-        <v>0.77388100000000004</v>
+        <v>0.75022</v>
       </c>
       <c r="H34">
-        <v>1.0164899999999999</v>
+        <v>1.0186200000000001</v>
       </c>
       <c r="I34">
-        <v>0.9476</v>
+        <v>0.90344999999999998</v>
       </c>
       <c r="J34">
-        <v>0.47299999999999998</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -14244,7 +14298,7 @@
         <v>0.9476</v>
       </c>
       <c r="J35">
-        <v>0.48599999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -14279,7 +14333,7 @@
         <v>0.9476</v>
       </c>
       <c r="J36">
-        <v>0.47799999999999998</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -14287,10 +14341,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>1682</v>
@@ -14299,22 +14353,22 @@
         <v>1000</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G37">
-        <v>0.70620000000000005</v>
+        <v>0.77388100000000004</v>
       </c>
       <c r="H37">
-        <v>1.01474</v>
+        <v>1.0164899999999999</v>
       </c>
       <c r="I37">
-        <v>0.82894999999999996</v>
+        <v>0.9476</v>
       </c>
       <c r="J37">
-        <v>0.438</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -14349,7 +14403,7 @@
         <v>0.82894999999999996</v>
       </c>
       <c r="J38">
-        <v>0.432</v>
+        <v>0.438</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -14384,7 +14438,7 @@
         <v>0.82894999999999996</v>
       </c>
       <c r="J39">
-        <v>0.45400000000000001</v>
+        <v>0.432</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -14392,7 +14446,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -14410,16 +14464,16 @@
         <v>13</v>
       </c>
       <c r="G40">
-        <v>0.75182599999999999</v>
+        <v>0.70620000000000005</v>
       </c>
       <c r="H40">
-        <v>1.02033</v>
+        <v>1.01474</v>
       </c>
       <c r="I40">
-        <v>0.90915000000000001</v>
+        <v>0.82894999999999996</v>
       </c>
       <c r="J40">
-        <v>0.48199999999999998</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -14454,7 +14508,7 @@
         <v>0.90915000000000001</v>
       </c>
       <c r="J41">
-        <v>0.47899999999999998</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="K41">
         <v>0</v>
@@ -14489,7 +14543,7 @@
         <v>0.90915000000000001</v>
       </c>
       <c r="J42">
-        <v>0.48499999999999999</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -14497,7 +14551,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -14515,16 +14569,16 @@
         <v>13</v>
       </c>
       <c r="G43">
-        <v>0.76868499999999995</v>
+        <v>0.75182599999999999</v>
       </c>
       <c r="H43">
-        <v>1.00787</v>
+        <v>1.02033</v>
       </c>
       <c r="I43">
-        <v>0.95379999999999998</v>
+        <v>0.90915000000000001</v>
       </c>
       <c r="J43">
-        <v>0.51400000000000001</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -14559,7 +14613,7 @@
         <v>0.95379999999999998</v>
       </c>
       <c r="J44">
-        <v>0.51200000000000001</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -14594,7 +14648,7 @@
         <v>0.95379999999999998</v>
       </c>
       <c r="J45">
-        <v>0.51800000000000002</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -14602,10 +14656,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>1682</v>
@@ -14620,16 +14674,16 @@
         <v>13</v>
       </c>
       <c r="G46">
-        <v>0.22004399999999999</v>
+        <v>0.76868499999999995</v>
       </c>
       <c r="H46">
-        <v>0.61187899999999995</v>
+        <v>1.00787</v>
       </c>
       <c r="I46">
-        <v>0.24049999999999999</v>
+        <v>0.95379999999999998</v>
       </c>
       <c r="J46">
-        <v>0.39200000000000002</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -14664,7 +14718,7 @@
         <v>0.24049999999999999</v>
       </c>
       <c r="J47">
-        <v>0.38700000000000001</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -14699,7 +14753,7 @@
         <v>0.24049999999999999</v>
       </c>
       <c r="J48">
-        <v>0.40600000000000003</v>
+        <v>0.38700000000000001</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -14707,7 +14761,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -14725,16 +14779,16 @@
         <v>13</v>
       </c>
       <c r="G49">
-        <v>0.29616799999999999</v>
+        <v>0.22004399999999999</v>
       </c>
       <c r="H49">
-        <v>0.70046799999999998</v>
+        <v>0.61187899999999995</v>
       </c>
       <c r="I49">
-        <v>0.32135000000000002</v>
+        <v>0.24049999999999999</v>
       </c>
       <c r="J49">
-        <v>0.439</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="K49">
         <v>0</v>
@@ -14769,7 +14823,7 @@
         <v>0.32135000000000002</v>
       </c>
       <c r="J50">
-        <v>0.45400000000000001</v>
+        <v>0.439</v>
       </c>
       <c r="K50">
         <v>0</v>
@@ -14804,7 +14858,7 @@
         <v>0.32135000000000002</v>
       </c>
       <c r="J51">
-        <v>0.42399999999999999</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -14812,7 +14866,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -14830,16 +14884,16 @@
         <v>13</v>
       </c>
       <c r="G52">
-        <v>0.38687700000000003</v>
+        <v>0.29616799999999999</v>
       </c>
       <c r="H52">
-        <v>0.79290300000000002</v>
+        <v>0.70046799999999998</v>
       </c>
       <c r="I52">
-        <v>0.41689999999999999</v>
+        <v>0.32135000000000002</v>
       </c>
       <c r="J52">
-        <v>0.40300000000000002</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -14874,7 +14928,7 @@
         <v>0.41689999999999999</v>
       </c>
       <c r="J53">
-        <v>0.46500000000000002</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -14909,7 +14963,7 @@
         <v>0.41689999999999999</v>
       </c>
       <c r="J54">
-        <v>0.46700000000000003</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K54">
         <v>0</v>
@@ -14917,10 +14971,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>1682</v>
@@ -14935,16 +14989,16 @@
         <v>13</v>
       </c>
       <c r="G55">
-        <v>0.24099799999999999</v>
+        <v>0.38687700000000003</v>
       </c>
       <c r="H55">
-        <v>0.63701099999999999</v>
+        <v>0.79290300000000002</v>
       </c>
       <c r="I55">
-        <v>0.24679999999999999</v>
+        <v>0.41689999999999999</v>
       </c>
       <c r="J55">
-        <v>0.44500000000000001</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -14979,7 +15033,7 @@
         <v>0.24679999999999999</v>
       </c>
       <c r="J56">
-        <v>0.42599999999999999</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -15014,7 +15068,7 @@
         <v>0.24679999999999999</v>
       </c>
       <c r="J57">
-        <v>0.42899999999999999</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -15022,7 +15076,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -15040,16 +15094,16 @@
         <v>13</v>
       </c>
       <c r="G58">
-        <v>0.32473600000000002</v>
+        <v>0.24099799999999999</v>
       </c>
       <c r="H58">
-        <v>0.73283900000000002</v>
+        <v>0.63701099999999999</v>
       </c>
       <c r="I58">
-        <v>0.32990000000000003</v>
+        <v>0.24679999999999999</v>
       </c>
       <c r="J58">
-        <v>0.40500000000000003</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="K58">
         <v>0</v>
@@ -15084,7 +15138,7 @@
         <v>0.32990000000000003</v>
       </c>
       <c r="J59">
-        <v>0.39300000000000002</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="K59">
         <v>0</v>
@@ -15119,7 +15173,7 @@
         <v>0.32990000000000003</v>
       </c>
       <c r="J60">
-        <v>0.4</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -15127,7 +15181,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -15145,16 +15199,16 @@
         <v>13</v>
       </c>
       <c r="G61">
-        <v>0.40194999999999997</v>
+        <v>0.32473600000000002</v>
       </c>
       <c r="H61">
-        <v>0.80304900000000001</v>
+        <v>0.73283900000000002</v>
       </c>
       <c r="I61">
-        <v>0.42049999999999998</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="J61">
-        <v>0.42199999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -15189,7 +15243,7 @@
         <v>0.42049999999999998</v>
       </c>
       <c r="J62">
-        <v>0.436</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -15224,7 +15278,7 @@
         <v>0.42049999999999998</v>
       </c>
       <c r="J63">
-        <v>0.40200000000000002</v>
+        <v>0.436</v>
       </c>
       <c r="K63">
         <v>0</v>
@@ -15232,10 +15286,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>1682</v>
@@ -15250,16 +15304,16 @@
         <v>13</v>
       </c>
       <c r="G64">
-        <v>0.67131799999999997</v>
+        <v>0.40194999999999997</v>
       </c>
       <c r="H64">
-        <v>0.99054500000000001</v>
+        <v>0.80304900000000001</v>
       </c>
       <c r="I64">
-        <v>0.78895000000000004</v>
+        <v>0.42049999999999998</v>
       </c>
       <c r="J64">
-        <v>0.42199999999999999</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="K64">
         <v>0</v>
@@ -15294,7 +15348,7 @@
         <v>0.78895000000000004</v>
       </c>
       <c r="J65">
-        <v>0.41799999999999998</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="K65">
         <v>0</v>
@@ -15329,7 +15383,7 @@
         <v>0.78895000000000004</v>
       </c>
       <c r="J66">
-        <v>0.40899999999999997</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="K66">
         <v>0</v>
@@ -15337,7 +15391,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -15355,16 +15409,16 @@
         <v>13</v>
       </c>
       <c r="G67">
-        <v>0.73373999999999995</v>
+        <v>0.67131799999999997</v>
       </c>
       <c r="H67">
-        <v>1.01363</v>
+        <v>0.99054500000000001</v>
       </c>
       <c r="I67">
-        <v>0.88219999999999998</v>
+        <v>0.78895000000000004</v>
       </c>
       <c r="J67">
-        <v>0.45900000000000002</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -15399,7 +15453,7 @@
         <v>0.88219999999999998</v>
       </c>
       <c r="J68">
-        <v>0.48799999999999999</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K68">
         <v>0</v>
@@ -15434,7 +15488,7 @@
         <v>0.88219999999999998</v>
       </c>
       <c r="J69">
-        <v>0.46899999999999997</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="K69">
         <v>0</v>
@@ -15442,7 +15496,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -15460,16 +15514,16 @@
         <v>13</v>
       </c>
       <c r="G70">
-        <v>0.76240300000000005</v>
+        <v>0.73373999999999995</v>
       </c>
       <c r="H70">
-        <v>1.0094700000000001</v>
+        <v>1.01363</v>
       </c>
       <c r="I70">
-        <v>0.94055</v>
+        <v>0.88219999999999998</v>
       </c>
       <c r="J70">
-        <v>0.57499999999999996</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="K70">
         <v>0</v>
@@ -15504,7 +15558,7 @@
         <v>0.94055</v>
       </c>
       <c r="J71">
-        <v>0.56799999999999995</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -15539,7 +15593,7 @@
         <v>0.94055</v>
       </c>
       <c r="J72">
-        <v>0.501</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="K72">
         <v>0</v>
@@ -15547,10 +15601,10 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C73">
         <v>1682</v>
@@ -15559,22 +15613,22 @@
         <v>1000</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F73" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G73">
-        <v>0.70508199999999999</v>
+        <v>0.76240300000000005</v>
       </c>
       <c r="H73">
-        <v>1.0118400000000001</v>
+        <v>1.0094700000000001</v>
       </c>
       <c r="I73">
-        <v>0.83035000000000003</v>
+        <v>0.94055</v>
       </c>
       <c r="J73">
-        <v>0.46500000000000002</v>
+        <v>0.501</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -15609,7 +15663,7 @@
         <v>0.83035000000000003</v>
       </c>
       <c r="J74">
-        <v>0.47599999999999998</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K74">
         <v>0</v>
@@ -15644,7 +15698,7 @@
         <v>0.83035000000000003</v>
       </c>
       <c r="J75">
-        <v>0.44600000000000001</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="K75">
         <v>0</v>
@@ -15652,7 +15706,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -15670,16 +15724,16 @@
         <v>15</v>
       </c>
       <c r="G76">
-        <v>0.75651100000000004</v>
+        <v>0.70508199999999999</v>
       </c>
       <c r="H76">
-        <v>1.02495</v>
+        <v>1.0118400000000001</v>
       </c>
       <c r="I76">
-        <v>0.91244999999999998</v>
+        <v>0.83035000000000003</v>
       </c>
       <c r="J76">
-        <v>0.45600000000000002</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="K76">
         <v>0</v>
@@ -15714,7 +15768,7 @@
         <v>0.91244999999999998</v>
       </c>
       <c r="J77">
-        <v>0.505</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K77">
         <v>0</v>
@@ -15749,7 +15803,7 @@
         <v>0.91244999999999998</v>
       </c>
       <c r="J78">
-        <v>0.46800000000000003</v>
+        <v>0.505</v>
       </c>
       <c r="K78">
         <v>0</v>
@@ -15757,7 +15811,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -15775,16 +15829,16 @@
         <v>15</v>
       </c>
       <c r="G79">
-        <v>0.77482700000000004</v>
+        <v>0.75651100000000004</v>
       </c>
       <c r="H79">
-        <v>1.0172600000000001</v>
+        <v>1.02495</v>
       </c>
       <c r="I79">
-        <v>0.95855000000000001</v>
+        <v>0.91244999999999998</v>
       </c>
       <c r="J79">
-        <v>0.56100000000000005</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="K79">
         <v>0</v>
@@ -15854,7 +15908,7 @@
         <v>0.95855000000000001</v>
       </c>
       <c r="J81">
-        <v>0.58199999999999996</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="K81">
         <v>0</v>
@@ -15862,10 +15916,10 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>1682</v>
@@ -15880,16 +15934,16 @@
         <v>15</v>
       </c>
       <c r="G82">
-        <v>0.22381799999999999</v>
+        <v>0.77482700000000004</v>
       </c>
       <c r="H82">
-        <v>0.63045399999999996</v>
+        <v>1.0172600000000001</v>
       </c>
       <c r="I82">
-        <v>0.22575000000000001</v>
+        <v>0.95855000000000001</v>
       </c>
       <c r="J82">
-        <v>0.48199999999999998</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="K82">
         <v>0</v>
@@ -15924,7 +15978,7 @@
         <v>0.22575000000000001</v>
       </c>
       <c r="J83">
-        <v>0.5</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="K83">
         <v>0</v>
@@ -15959,7 +16013,7 @@
         <v>0.22575000000000001</v>
       </c>
       <c r="J84">
-        <v>0.48</v>
+        <v>0.5</v>
       </c>
       <c r="K84">
         <v>0</v>
@@ -15967,7 +16021,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -15985,16 +16039,16 @@
         <v>15</v>
       </c>
       <c r="G85">
-        <v>0.32249800000000001</v>
+        <v>0.22381799999999999</v>
       </c>
       <c r="H85">
-        <v>0.73726000000000003</v>
+        <v>0.63045399999999996</v>
       </c>
       <c r="I85">
-        <v>0.33200000000000002</v>
+        <v>0.22575000000000001</v>
       </c>
       <c r="J85">
-        <v>0.46300000000000002</v>
+        <v>0.48</v>
       </c>
       <c r="K85">
         <v>0</v>
@@ -16029,7 +16083,7 @@
         <v>0.33200000000000002</v>
       </c>
       <c r="J86">
-        <v>0.47699999999999998</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="K86">
         <v>0</v>
@@ -16064,7 +16118,7 @@
         <v>0.33200000000000002</v>
       </c>
       <c r="J87">
-        <v>0.48899999999999999</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="K87">
         <v>0</v>
@@ -16072,7 +16126,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -16090,16 +16144,16 @@
         <v>15</v>
       </c>
       <c r="G88">
-        <v>0.41699000000000003</v>
+        <v>0.32249800000000001</v>
       </c>
       <c r="H88">
-        <v>0.82313400000000003</v>
+        <v>0.73726000000000003</v>
       </c>
       <c r="I88">
-        <v>0.43540000000000001</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="J88">
-        <v>0.48</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="K88">
         <v>0</v>
@@ -16134,7 +16188,7 @@
         <v>0.43540000000000001</v>
       </c>
       <c r="J89">
-        <v>0.44900000000000001</v>
+        <v>0.48</v>
       </c>
       <c r="K89">
         <v>0</v>
@@ -16169,7 +16223,7 @@
         <v>0.43540000000000001</v>
       </c>
       <c r="J90">
-        <v>0.52600000000000002</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="K90">
         <v>0</v>
@@ -16177,10 +16231,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>1682</v>
@@ -16195,16 +16249,16 @@
         <v>15</v>
       </c>
       <c r="G91">
-        <v>0.24574799999999999</v>
+        <v>0.41699000000000003</v>
       </c>
       <c r="H91">
-        <v>0.66067500000000001</v>
+        <v>0.82313400000000003</v>
       </c>
       <c r="I91">
-        <v>0.23125000000000001</v>
+        <v>0.43540000000000001</v>
       </c>
       <c r="J91">
-        <v>0.5</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="K91">
         <v>0</v>
@@ -16239,7 +16293,7 @@
         <v>0.23125000000000001</v>
       </c>
       <c r="J92">
-        <v>0.51200000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="K92">
         <v>0</v>
@@ -16274,7 +16328,7 @@
         <v>0.23125000000000001</v>
       </c>
       <c r="J93">
-        <v>0.45800000000000002</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="K93">
         <v>0</v>
@@ -16282,7 +16336,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -16300,16 +16354,16 @@
         <v>15</v>
       </c>
       <c r="G94">
-        <v>0.34462100000000001</v>
+        <v>0.24574799999999999</v>
       </c>
       <c r="H94">
-        <v>0.76558099999999996</v>
+        <v>0.66067500000000001</v>
       </c>
       <c r="I94">
-        <v>0.33189999999999997</v>
+        <v>0.23125000000000001</v>
       </c>
       <c r="J94">
-        <v>0.46200000000000002</v>
+        <v>0.45800000000000002</v>
       </c>
       <c r="K94">
         <v>0</v>
@@ -16344,7 +16398,7 @@
         <v>0.33189999999999997</v>
       </c>
       <c r="J95">
-        <v>0.45</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="K95">
         <v>0</v>
@@ -16379,7 +16433,7 @@
         <v>0.33189999999999997</v>
       </c>
       <c r="J96">
-        <v>0.45400000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="K96">
         <v>0</v>
@@ -16387,7 +16441,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -16405,16 +16459,16 @@
         <v>15</v>
       </c>
       <c r="G97">
-        <v>0.432336</v>
+        <v>0.34462100000000001</v>
       </c>
       <c r="H97">
-        <v>0.84072800000000003</v>
+        <v>0.76558099999999996</v>
       </c>
       <c r="I97">
-        <v>0.42759999999999998</v>
+        <v>0.33189999999999997</v>
       </c>
       <c r="J97">
-        <v>0.47499999999999998</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="K97">
         <v>0</v>
@@ -16449,7 +16503,7 @@
         <v>0.42759999999999998</v>
       </c>
       <c r="J98">
-        <v>0.45500000000000002</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="K98">
         <v>0</v>
@@ -16484,7 +16538,7 @@
         <v>0.42759999999999998</v>
       </c>
       <c r="J99">
-        <v>0.49</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="K99">
         <v>0</v>
@@ -16492,10 +16546,10 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100">
         <v>1682</v>
@@ -16510,16 +16564,16 @@
         <v>15</v>
       </c>
       <c r="G100">
-        <v>0.67707499999999998</v>
+        <v>0.432336</v>
       </c>
       <c r="H100">
-        <v>0.99413799999999997</v>
+        <v>0.84072800000000003</v>
       </c>
       <c r="I100">
-        <v>0.79644999999999999</v>
+        <v>0.42759999999999998</v>
       </c>
       <c r="J100">
-        <v>0.48699999999999999</v>
+        <v>0.49</v>
       </c>
       <c r="K100">
         <v>0</v>
@@ -16554,7 +16608,7 @@
         <v>0.79644999999999999</v>
       </c>
       <c r="J101">
-        <v>0.50600000000000001</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="K101">
         <v>0</v>
@@ -16589,7 +16643,7 @@
         <v>0.79644999999999999</v>
       </c>
       <c r="J102">
-        <v>0.495</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="K102">
         <v>0</v>
@@ -16597,7 +16651,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -16615,16 +16669,16 @@
         <v>15</v>
       </c>
       <c r="G103">
-        <v>0.73651100000000003</v>
+        <v>0.67707499999999998</v>
       </c>
       <c r="H103">
-        <v>1.01149</v>
+        <v>0.99413799999999997</v>
       </c>
       <c r="I103">
-        <v>0.88980000000000004</v>
+        <v>0.79644999999999999</v>
       </c>
       <c r="J103">
-        <v>0.503</v>
+        <v>0.495</v>
       </c>
       <c r="K103">
         <v>0</v>
@@ -16659,7 +16713,7 @@
         <v>0.88980000000000004</v>
       </c>
       <c r="J104">
-        <v>0.505</v>
+        <v>0.503</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -16694,7 +16748,7 @@
         <v>0.88980000000000004</v>
       </c>
       <c r="J105">
-        <v>0.53400000000000003</v>
+        <v>0.505</v>
       </c>
       <c r="K105">
         <v>0</v>
@@ -16702,7 +16756,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -16720,16 +16774,16 @@
         <v>15</v>
       </c>
       <c r="G106">
-        <v>0.76467200000000002</v>
+        <v>0.73651100000000003</v>
       </c>
       <c r="H106">
-        <v>1.01441</v>
+        <v>1.01149</v>
       </c>
       <c r="I106">
-        <v>0.94415000000000004</v>
+        <v>0.88980000000000004</v>
       </c>
       <c r="J106">
-        <v>0.56699999999999995</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="K106">
         <v>0</v>
@@ -16764,7 +16818,7 @@
         <v>0.94415000000000004</v>
       </c>
       <c r="J107">
-        <v>0.504</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="K107">
         <v>0</v>
@@ -16799,7 +16853,7 @@
         <v>0.94415000000000004</v>
       </c>
       <c r="J108">
-        <v>0.52500000000000002</v>
+        <v>0.504</v>
       </c>
       <c r="K108">
         <v>0</v>
@@ -16807,10 +16861,10 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C109">
         <v>1682</v>
@@ -16819,22 +16873,22 @@
         <v>1000</v>
       </c>
       <c r="E109" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G109">
-        <v>0.71483799999999997</v>
+        <v>0.76467200000000002</v>
       </c>
       <c r="H109">
-        <v>1.0278</v>
+        <v>1.01441</v>
       </c>
       <c r="I109">
-        <v>0.83245000000000002</v>
+        <v>0.94415000000000004</v>
       </c>
       <c r="J109">
-        <v>0.48099999999999998</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="K109">
         <v>0</v>
@@ -16869,7 +16923,7 @@
         <v>0.83245000000000002</v>
       </c>
       <c r="J110">
-        <v>0.46899999999999997</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -16904,7 +16958,7 @@
         <v>0.83245000000000002</v>
       </c>
       <c r="J111">
-        <v>0.505</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="K111">
         <v>0</v>
@@ -16912,7 +16966,7 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -16930,16 +16984,16 @@
         <v>17</v>
       </c>
       <c r="G112">
-        <v>0.75752900000000001</v>
+        <v>0.71483799999999997</v>
       </c>
       <c r="H112">
-        <v>1.0241199999999999</v>
+        <v>1.0278</v>
       </c>
       <c r="I112">
-        <v>0.91149999999999998</v>
+        <v>0.83245000000000002</v>
       </c>
       <c r="J112">
-        <v>0.50900000000000001</v>
+        <v>0.505</v>
       </c>
       <c r="K112">
         <v>0</v>
@@ -16974,7 +17028,7 @@
         <v>0.91149999999999998</v>
       </c>
       <c r="J113">
-        <v>0.46200000000000002</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="K113">
         <v>0</v>
@@ -17009,7 +17063,7 @@
         <v>0.91149999999999998</v>
       </c>
       <c r="J114">
-        <v>0.48</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="K114">
         <v>0</v>
@@ -17017,7 +17071,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -17035,16 +17089,16 @@
         <v>17</v>
       </c>
       <c r="G115">
-        <v>0.78012400000000004</v>
+        <v>0.75752900000000001</v>
       </c>
       <c r="H115">
-        <v>1.0210999999999999</v>
+        <v>1.0241199999999999</v>
       </c>
       <c r="I115">
-        <v>0.95760000000000001</v>
+        <v>0.91149999999999998</v>
       </c>
       <c r="J115">
-        <v>0.57599999999999996</v>
+        <v>0.48</v>
       </c>
       <c r="K115">
         <v>0</v>
@@ -17079,7 +17133,7 @@
         <v>0.95760000000000001</v>
       </c>
       <c r="J116">
-        <v>0.54800000000000004</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="K116">
         <v>0</v>
@@ -17114,7 +17168,7 @@
         <v>0.95760000000000001</v>
       </c>
       <c r="J117">
-        <v>0.55800000000000005</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="K117">
         <v>0</v>
@@ -17122,10 +17176,10 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C118">
         <v>1682</v>
@@ -17140,16 +17194,16 @@
         <v>17</v>
       </c>
       <c r="G118">
-        <v>0.19620899999999999</v>
+        <v>0.78012400000000004</v>
       </c>
       <c r="H118">
-        <v>0.56994500000000003</v>
+        <v>1.0210999999999999</v>
       </c>
       <c r="I118">
-        <v>0.21229999999999999</v>
+        <v>0.95760000000000001</v>
       </c>
       <c r="J118">
-        <v>0.49299999999999999</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="K118">
         <v>0</v>
@@ -17184,7 +17238,7 @@
         <v>0.21229999999999999</v>
       </c>
       <c r="J119">
-        <v>0.47399999999999998</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="K119">
         <v>0</v>
@@ -17219,7 +17273,7 @@
         <v>0.21229999999999999</v>
       </c>
       <c r="J120">
-        <v>0.46100000000000002</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="K120">
         <v>0</v>
@@ -17227,7 +17281,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -17245,16 +17299,16 @@
         <v>17</v>
       </c>
       <c r="G121">
-        <v>0.27655000000000002</v>
+        <v>0.19620899999999999</v>
       </c>
       <c r="H121">
-        <v>0.66312899999999997</v>
+        <v>0.56994500000000003</v>
       </c>
       <c r="I121">
-        <v>0.30409999999999998</v>
+        <v>0.21229999999999999</v>
       </c>
       <c r="J121">
-        <v>0.46600000000000003</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="K121">
         <v>0</v>
@@ -17289,7 +17343,7 @@
         <v>0.30409999999999998</v>
       </c>
       <c r="J122">
-        <v>0.48799999999999999</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="K122">
         <v>0</v>
@@ -17324,7 +17378,7 @@
         <v>0.30409999999999998</v>
       </c>
       <c r="J123">
-        <v>0.46500000000000002</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="K123">
         <v>0</v>
@@ -17332,7 +17386,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -17350,16 +17404,16 @@
         <v>17</v>
       </c>
       <c r="G124">
-        <v>0.37776599999999999</v>
+        <v>0.27655000000000002</v>
       </c>
       <c r="H124">
-        <v>0.77344000000000002</v>
+        <v>0.66312899999999997</v>
       </c>
       <c r="I124">
-        <v>0.40960000000000002</v>
+        <v>0.30409999999999998</v>
       </c>
       <c r="J124">
-        <v>0.51300000000000001</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K124">
         <v>0</v>
@@ -17394,7 +17448,7 @@
         <v>0.40960000000000002</v>
       </c>
       <c r="J125">
-        <v>0.45300000000000001</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="K125">
         <v>0</v>
@@ -17429,7 +17483,7 @@
         <v>0.40960000000000002</v>
       </c>
       <c r="J126">
-        <v>0.46500000000000002</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="K126">
         <v>0</v>
@@ -17437,10 +17491,10 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C127">
         <v>1682</v>
@@ -17455,16 +17509,16 @@
         <v>17</v>
       </c>
       <c r="G127">
-        <v>0.22196399999999999</v>
+        <v>0.37776599999999999</v>
       </c>
       <c r="H127">
-        <v>0.61735099999999998</v>
+        <v>0.77344000000000002</v>
       </c>
       <c r="I127">
-        <v>0.21625</v>
+        <v>0.40960000000000002</v>
       </c>
       <c r="J127">
-        <v>0.48399999999999999</v>
+        <v>0.46500000000000002</v>
       </c>
       <c r="K127">
         <v>0</v>
@@ -17499,7 +17553,7 @@
         <v>0.21625</v>
       </c>
       <c r="J128">
-        <v>0.49</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="K128">
         <v>0</v>
@@ -17534,7 +17588,7 @@
         <v>0.21625</v>
       </c>
       <c r="J129">
-        <v>0.44900000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="K129">
         <v>0</v>
@@ -17542,7 +17596,7 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B130">
         <v>2</v>
@@ -17560,16 +17614,16 @@
         <v>17</v>
       </c>
       <c r="G130">
-        <v>0.305898</v>
+        <v>0.22196399999999999</v>
       </c>
       <c r="H130">
-        <v>0.701901</v>
+        <v>0.61735099999999998</v>
       </c>
       <c r="I130">
-        <v>0.31485000000000002</v>
+        <v>0.21625</v>
       </c>
       <c r="J130">
-        <v>0.46100000000000002</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="K130">
         <v>0</v>
@@ -17604,7 +17658,7 @@
         <v>0.31485000000000002</v>
       </c>
       <c r="J131">
-        <v>0.48199999999999998</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="K131">
         <v>0</v>
@@ -17639,7 +17693,7 @@
         <v>0.31485000000000002</v>
       </c>
       <c r="J132">
-        <v>0.443</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="K132">
         <v>0</v>
@@ -17647,7 +17701,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B133">
         <v>2</v>
@@ -17665,16 +17719,16 @@
         <v>17</v>
       </c>
       <c r="G133">
-        <v>0.40614</v>
+        <v>0.305898</v>
       </c>
       <c r="H133">
-        <v>0.80742899999999995</v>
+        <v>0.701901</v>
       </c>
       <c r="I133">
-        <v>0.41610000000000003</v>
+        <v>0.31485000000000002</v>
       </c>
       <c r="J133">
-        <v>0.48</v>
+        <v>0.443</v>
       </c>
       <c r="K133">
         <v>0</v>
@@ -17709,7 +17763,7 @@
         <v>0.41610000000000003</v>
       </c>
       <c r="J134">
-        <v>0.502</v>
+        <v>0.48</v>
       </c>
       <c r="K134">
         <v>0</v>
@@ -17744,7 +17798,7 @@
         <v>0.41610000000000003</v>
       </c>
       <c r="J135">
-        <v>0.48499999999999999</v>
+        <v>0.502</v>
       </c>
       <c r="K135">
         <v>0</v>
@@ -17752,10 +17806,10 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B136">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136">
         <v>1682</v>
@@ -17770,16 +17824,16 @@
         <v>17</v>
       </c>
       <c r="G136">
-        <v>0.67281100000000005</v>
+        <v>0.40614</v>
       </c>
       <c r="H136">
-        <v>0.99746400000000002</v>
+        <v>0.80742899999999995</v>
       </c>
       <c r="I136">
-        <v>0.78785000000000005</v>
+        <v>0.41610000000000003</v>
       </c>
       <c r="J136">
-        <v>0.48799999999999999</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="K136">
         <v>0</v>
@@ -17814,7 +17868,7 @@
         <v>0.78785000000000005</v>
       </c>
       <c r="J137">
-        <v>0.48699999999999999</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="K137">
         <v>0</v>
@@ -17849,7 +17903,7 @@
         <v>0.78785000000000005</v>
       </c>
       <c r="J138">
-        <v>0.47</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="K138">
         <v>0</v>
@@ -17857,7 +17911,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B139">
         <v>3</v>
@@ -17875,16 +17929,16 @@
         <v>17</v>
       </c>
       <c r="G139">
-        <v>0.73698799999999998</v>
+        <v>0.67281100000000005</v>
       </c>
       <c r="H139">
-        <v>1.01451</v>
+        <v>0.99746400000000002</v>
       </c>
       <c r="I139">
-        <v>0.88600000000000001</v>
+        <v>0.78785000000000005</v>
       </c>
       <c r="J139">
-        <v>0.59199999999999997</v>
+        <v>0.47</v>
       </c>
       <c r="K139">
         <v>0</v>
@@ -17919,7 +17973,7 @@
         <v>0.88600000000000001</v>
       </c>
       <c r="J140">
-        <v>0.55000000000000004</v>
+        <v>0.59199999999999997</v>
       </c>
       <c r="K140">
         <v>0</v>
@@ -17954,7 +18008,7 @@
         <v>0.88600000000000001</v>
       </c>
       <c r="J141">
-        <v>0.54300000000000004</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K141">
         <v>0</v>
@@ -17962,7 +18016,7 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B142">
         <v>3</v>
@@ -17980,16 +18034,16 @@
         <v>17</v>
       </c>
       <c r="G142">
-        <v>0.76687799999999995</v>
+        <v>0.73698799999999998</v>
       </c>
       <c r="H142">
-        <v>1.0135700000000001</v>
+        <v>1.01451</v>
       </c>
       <c r="I142">
-        <v>0.94259999999999999</v>
+        <v>0.88600000000000001</v>
       </c>
       <c r="J142">
-        <v>0.60799999999999998</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="K142">
         <v>0</v>
@@ -18024,7 +18078,7 @@
         <v>0.94259999999999999</v>
       </c>
       <c r="J143">
-        <v>0.621</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="K143">
         <v>0</v>
@@ -18059,7 +18113,7 @@
         <v>0.94259999999999999</v>
       </c>
       <c r="J144">
-        <v>0.64100000000000001</v>
+        <v>0.621</v>
       </c>
       <c r="K144">
         <v>0</v>
@@ -18067,10 +18121,10 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C145">
         <v>1682</v>
@@ -18079,22 +18133,22 @@
         <v>1000</v>
       </c>
       <c r="E145" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F145" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G145">
-        <v>0.70908599999999999</v>
+        <v>0.76687799999999995</v>
       </c>
       <c r="H145">
-        <v>1.0130399999999999</v>
+        <v>1.0135700000000001</v>
       </c>
       <c r="I145">
-        <v>0.83835000000000004</v>
+        <v>0.94259999999999999</v>
       </c>
       <c r="J145">
-        <v>0.55700000000000005</v>
+        <v>0.64100000000000001</v>
       </c>
       <c r="K145">
         <v>0</v>
@@ -18129,7 +18183,7 @@
         <v>0.83835000000000004</v>
       </c>
       <c r="J146">
-        <v>0.56299999999999994</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="K146">
         <v>0</v>
@@ -18164,7 +18218,7 @@
         <v>0.83835000000000004</v>
       </c>
       <c r="J147">
-        <v>0.54</v>
+        <v>0.56299999999999994</v>
       </c>
       <c r="K147">
         <v>0</v>
@@ -18172,7 +18226,7 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -18190,16 +18244,16 @@
         <v>19</v>
       </c>
       <c r="G148">
-        <v>0.75605</v>
+        <v>0.70908599999999999</v>
       </c>
       <c r="H148">
-        <v>1.0207999999999999</v>
+        <v>1.0130399999999999</v>
       </c>
       <c r="I148">
-        <v>0.91695000000000004</v>
+        <v>0.83835000000000004</v>
       </c>
       <c r="J148">
-        <v>0.51300000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="K148">
         <v>0</v>
@@ -18234,7 +18288,7 @@
         <v>0.91695000000000004</v>
       </c>
       <c r="J149">
-        <v>0.49299999999999999</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="K149">
         <v>0</v>
@@ -18269,7 +18323,7 @@
         <v>0.91695000000000004</v>
       </c>
       <c r="J150">
-        <v>0.47199999999999998</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="K150">
         <v>0</v>
@@ -18277,7 +18331,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -18295,16 +18349,16 @@
         <v>19</v>
       </c>
       <c r="G151">
-        <v>0.77903299999999998</v>
+        <v>0.75605</v>
       </c>
       <c r="H151">
-        <v>1.01928</v>
+        <v>1.0207999999999999</v>
       </c>
       <c r="I151">
-        <v>0.96040000000000003</v>
+        <v>0.91695000000000004</v>
       </c>
       <c r="J151">
-        <v>0.55500000000000005</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="K151">
         <v>0</v>
@@ -18339,7 +18393,7 @@
         <v>0.96040000000000003</v>
       </c>
       <c r="J152">
-        <v>0.56899999999999995</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -18374,7 +18428,7 @@
         <v>0.96040000000000003</v>
       </c>
       <c r="J153">
-        <v>0.54300000000000004</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -18382,10 +18436,10 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C154">
         <v>1682</v>
@@ -18400,16 +18454,16 @@
         <v>19</v>
       </c>
       <c r="G154">
-        <v>0.18532299999999999</v>
+        <v>0.77903299999999998</v>
       </c>
       <c r="H154">
-        <v>0.54721699999999995</v>
+        <v>1.01928</v>
       </c>
       <c r="I154">
-        <v>0.20580000000000001</v>
+        <v>0.96040000000000003</v>
       </c>
       <c r="J154">
-        <v>0.438</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="K154">
         <v>0</v>
@@ -18444,7 +18498,7 @@
         <v>0.20580000000000001</v>
       </c>
       <c r="J155">
-        <v>0.46600000000000003</v>
+        <v>0.438</v>
       </c>
       <c r="K155">
         <v>0</v>
@@ -18479,7 +18533,7 @@
         <v>0.20580000000000001</v>
       </c>
       <c r="J156">
-        <v>0.44</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="K156">
         <v>0</v>
@@ -18487,7 +18541,7 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -18505,16 +18559,16 @@
         <v>19</v>
       </c>
       <c r="G157">
-        <v>0.27379999999999999</v>
+        <v>0.18532299999999999</v>
       </c>
       <c r="H157">
-        <v>0.65809799999999996</v>
+        <v>0.54721699999999995</v>
       </c>
       <c r="I157">
-        <v>0.30099999999999999</v>
+        <v>0.20580000000000001</v>
       </c>
       <c r="J157">
-        <v>0.44400000000000001</v>
+        <v>0.44</v>
       </c>
       <c r="K157">
         <v>0</v>
@@ -18549,7 +18603,7 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="J158">
-        <v>0.505</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="K158">
         <v>0</v>
@@ -18584,7 +18638,7 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="J159">
-        <v>0.44900000000000001</v>
+        <v>0.505</v>
       </c>
       <c r="K159">
         <v>0</v>
@@ -18592,7 +18646,7 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -18610,16 +18664,16 @@
         <v>19</v>
       </c>
       <c r="G160">
-        <v>0.36151800000000001</v>
+        <v>0.27379999999999999</v>
       </c>
       <c r="H160">
-        <v>0.75155300000000003</v>
+        <v>0.65809799999999996</v>
       </c>
       <c r="I160">
-        <v>0.39889999999999998</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="J160">
-        <v>0.439</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="K160">
         <v>0</v>
@@ -18654,7 +18708,7 @@
         <v>0.39889999999999998</v>
       </c>
       <c r="J161">
-        <v>0.504</v>
+        <v>0.439</v>
       </c>
       <c r="K161">
         <v>0</v>
@@ -18689,7 +18743,7 @@
         <v>0.39889999999999998</v>
       </c>
       <c r="J162">
-        <v>0.47</v>
+        <v>0.504</v>
       </c>
       <c r="K162">
         <v>0</v>
@@ -18697,10 +18751,10 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C163">
         <v>1682</v>
@@ -18715,16 +18769,16 @@
         <v>19</v>
       </c>
       <c r="G163">
-        <v>0.22337199999999999</v>
+        <v>0.36151800000000001</v>
       </c>
       <c r="H163">
-        <v>0.60535799999999995</v>
+        <v>0.75155300000000003</v>
       </c>
       <c r="I163">
-        <v>0.2283</v>
+        <v>0.39889999999999998</v>
       </c>
       <c r="J163">
-        <v>0.47499999999999998</v>
+        <v>0.47</v>
       </c>
       <c r="K163">
         <v>0</v>
@@ -18759,7 +18813,7 @@
         <v>0.2283</v>
       </c>
       <c r="J164">
-        <v>0.51400000000000001</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="K164">
         <v>0</v>
@@ -18794,7 +18848,7 @@
         <v>0.2283</v>
       </c>
       <c r="J165">
-        <v>0.54400000000000004</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="K165">
         <v>0</v>
@@ -18802,7 +18856,7 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B166">
         <v>2</v>
@@ -18820,16 +18874,16 @@
         <v>19</v>
       </c>
       <c r="G166">
-        <v>0.31759700000000002</v>
+        <v>0.22337199999999999</v>
       </c>
       <c r="H166">
-        <v>0.71369000000000005</v>
+        <v>0.60535799999999995</v>
       </c>
       <c r="I166">
-        <v>0.32784999999999997</v>
+        <v>0.2283</v>
       </c>
       <c r="J166">
-        <v>0.53</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -18864,7 +18918,7 @@
         <v>0.32784999999999997</v>
       </c>
       <c r="J167">
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="K167">
         <v>0</v>
@@ -18899,7 +18953,7 @@
         <v>0.32784999999999997</v>
       </c>
       <c r="J168">
-        <v>0.45700000000000002</v>
+        <v>0.48</v>
       </c>
       <c r="K168">
         <v>0</v>
@@ -18907,7 +18961,7 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B169">
         <v>2</v>
@@ -18925,16 +18979,16 @@
         <v>19</v>
       </c>
       <c r="G169">
-        <v>0.40441199999999999</v>
+        <v>0.31759700000000002</v>
       </c>
       <c r="H169">
-        <v>0.80077399999999999</v>
+        <v>0.71369000000000005</v>
       </c>
       <c r="I169">
-        <v>0.42404999999999998</v>
+        <v>0.32784999999999997</v>
       </c>
       <c r="J169">
-        <v>0.499</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="K169">
         <v>0</v>
@@ -18969,7 +19023,7 @@
         <v>0.42404999999999998</v>
       </c>
       <c r="J170">
-        <v>0.45900000000000002</v>
+        <v>0.499</v>
       </c>
       <c r="K170">
         <v>0</v>
@@ -19004,7 +19058,7 @@
         <v>0.42404999999999998</v>
       </c>
       <c r="J171">
-        <v>0.61099999999999999</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="K171">
         <v>0</v>
@@ -19012,10 +19066,10 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B172">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172">
         <v>1682</v>
@@ -19030,16 +19084,16 @@
         <v>19</v>
       </c>
       <c r="G172">
-        <v>0.68130599999999997</v>
+        <v>0.40441199999999999</v>
       </c>
       <c r="H172">
-        <v>0.99735600000000002</v>
+        <v>0.80077399999999999</v>
       </c>
       <c r="I172">
-        <v>0.80389999999999995</v>
+        <v>0.42404999999999998</v>
       </c>
       <c r="J172">
-        <v>0.47799999999999998</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="K172">
         <v>0</v>
@@ -19074,7 +19128,7 @@
         <v>0.80389999999999995</v>
       </c>
       <c r="J173">
-        <v>0.51600000000000001</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="K173">
         <v>0</v>
@@ -19109,7 +19163,7 @@
         <v>0.80389999999999995</v>
       </c>
       <c r="J174">
-        <v>0.498</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="K174">
         <v>0</v>
@@ -19117,7 +19171,7 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B175">
         <v>3</v>
@@ -19135,16 +19189,16 @@
         <v>19</v>
       </c>
       <c r="G175">
-        <v>0.737016</v>
+        <v>0.68130599999999997</v>
       </c>
       <c r="H175">
-        <v>1.0107999999999999</v>
+        <v>0.99735600000000002</v>
       </c>
       <c r="I175">
-        <v>0.89475000000000005</v>
+        <v>0.80389999999999995</v>
       </c>
       <c r="J175">
-        <v>0.52800000000000002</v>
+        <v>0.498</v>
       </c>
       <c r="K175">
         <v>0</v>
@@ -19179,7 +19233,7 @@
         <v>0.89475000000000005</v>
       </c>
       <c r="J176">
-        <v>0.48899999999999999</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="K176">
         <v>0</v>
@@ -19214,7 +19268,7 @@
         <v>0.89475000000000005</v>
       </c>
       <c r="J177">
-        <v>0.51200000000000001</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="K177">
         <v>0</v>
@@ -19222,7 +19276,7 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B178">
         <v>3</v>
@@ -19240,16 +19294,16 @@
         <v>19</v>
       </c>
       <c r="G178">
-        <v>0.767119</v>
+        <v>0.737016</v>
       </c>
       <c r="H178">
-        <v>1.0112099999999999</v>
+        <v>1.0107999999999999</v>
       </c>
       <c r="I178">
-        <v>0.94564999999999999</v>
+        <v>0.89475000000000005</v>
       </c>
       <c r="J178">
-        <v>0.58499999999999996</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="K178">
         <v>0</v>
@@ -19284,7 +19338,7 @@
         <v>0.94564999999999999</v>
       </c>
       <c r="J179">
-        <v>0.55300000000000005</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="K179">
         <v>0</v>
@@ -19319,9 +19373,44 @@
         <v>0.94564999999999999</v>
       </c>
       <c r="J180">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="K180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>20</v>
+      </c>
+      <c r="B181">
+        <v>3</v>
+      </c>
+      <c r="C181">
+        <v>1682</v>
+      </c>
+      <c r="D181">
+        <v>1000</v>
+      </c>
+      <c r="E181" t="s">
+        <v>18</v>
+      </c>
+      <c r="F181" t="s">
+        <v>19</v>
+      </c>
+      <c r="G181">
+        <v>0.767119</v>
+      </c>
+      <c r="H181">
+        <v>1.0112099999999999</v>
+      </c>
+      <c r="I181">
+        <v>0.94564999999999999</v>
+      </c>
+      <c r="J181">
         <v>0.56799999999999995</v>
       </c>
-      <c r="K180">
+      <c r="K181">
         <v>0</v>
       </c>
     </row>
@@ -27011,8 +27100,8 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K181"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="K181" sqref="A2:K181"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27027,6 +27116,16 @@
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -27037,10 +27136,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>28</v>
@@ -27093,7 +27192,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J2">
-        <v>6.3529999999999998</v>
+        <v>4.4749999999999996</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -27128,7 +27227,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J3">
-        <v>6.6589999999999998</v>
+        <v>4.0709999999999997</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -27163,7 +27262,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J4">
-        <v>7.3049999999999997</v>
+        <v>4.0170000000000003</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -27198,7 +27297,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J5">
-        <v>6.7889999999999997</v>
+        <v>4.7949999999999999</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -27233,7 +27332,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J6">
-        <v>6.4829999999999997</v>
+        <v>5.2839999999999998</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -27268,7 +27367,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J7">
-        <v>6.2629999999999999</v>
+        <v>4.7779999999999996</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -27303,7 +27402,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J8">
-        <v>6.7060000000000004</v>
+        <v>4.0439999999999996</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -27338,7 +27437,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J9">
-        <v>6.3040000000000003</v>
+        <v>4.6310000000000002</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -27373,7 +27472,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J10">
-        <v>6.1349999999999998</v>
+        <v>4.6820000000000004</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -27408,7 +27507,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J11">
-        <v>6.2080000000000002</v>
+        <v>4.6829999999999998</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -27443,7 +27542,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J12">
-        <v>5.8869999999999996</v>
+        <v>4.2389999999999999</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -27478,7 +27577,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J13">
-        <v>5.8010000000000002</v>
+        <v>4.6070000000000002</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -27513,7 +27612,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J14">
-        <v>5.7469999999999999</v>
+        <v>3.8919999999999999</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -27548,7 +27647,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J15">
-        <v>5.7649999999999997</v>
+        <v>3.9430000000000001</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -27583,7 +27682,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J16">
-        <v>6.7160000000000002</v>
+        <v>3.698</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -27618,7 +27717,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J17">
-        <v>6.28</v>
+        <v>4.4459999999999997</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -27653,7 +27752,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J18">
-        <v>6.327</v>
+        <v>3.7130000000000001</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -27688,7 +27787,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J19">
-        <v>6.1369999999999996</v>
+        <v>3.6389999999999998</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -27723,7 +27822,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J20">
-        <v>6.4080000000000004</v>
+        <v>3.1960000000000002</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -27758,7 +27857,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J21">
-        <v>5.8019999999999996</v>
+        <v>3.86</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -27793,7 +27892,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J22">
-        <v>6.2729999999999997</v>
+        <v>3.1930000000000001</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -27828,7 +27927,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J23">
-        <v>6.1189999999999998</v>
+        <v>3.3919999999999999</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -27863,7 +27962,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J24">
-        <v>6.1509999999999998</v>
+        <v>3.9009999999999998</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -27898,7 +27997,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J25">
-        <v>5.7389999999999999</v>
+        <v>3.504</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -27933,7 +28032,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J26">
-        <v>5.6449999999999996</v>
+        <v>3.5750000000000002</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -27968,7 +28067,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J27">
-        <v>5.8650000000000002</v>
+        <v>3.84</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -28003,7 +28102,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J28">
-        <v>5.5609999999999999</v>
+        <v>3.7210000000000001</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -28038,7 +28137,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J29">
-        <v>5.6950000000000003</v>
+        <v>4.0810000000000004</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -28073,7 +28172,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J30">
-        <v>5.5960000000000001</v>
+        <v>4.4470000000000001</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -28108,7 +28207,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J31">
-        <v>5.7629999999999999</v>
+        <v>4.8860000000000001</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -28143,7 +28242,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J32">
-        <v>6.0289999999999999</v>
+        <v>4.5090000000000003</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -28178,7 +28277,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J33">
-        <v>5.7939999999999996</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -28213,7 +28312,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J34">
-        <v>6.1440000000000001</v>
+        <v>4.5970000000000004</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -28248,7 +28347,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J35">
-        <v>6.5759999999999996</v>
+        <v>4.67</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -28283,7 +28382,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J36">
-        <v>6.2519999999999998</v>
+        <v>4.66</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -28318,7 +28417,7 @@
         <v>0.99839999999999995</v>
       </c>
       <c r="J37">
-        <v>5.9450000000000003</v>
+        <v>4.7380000000000004</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -28353,7 +28452,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J38">
-        <v>5.5590000000000002</v>
+        <v>4.3140000000000001</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -28388,7 +28487,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J39">
-        <v>5.117</v>
+        <v>4.4630000000000001</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -28423,7 +28522,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J40">
-        <v>5.476</v>
+        <v>4.2229999999999999</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -28458,7 +28557,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J41">
-        <v>5.7380000000000004</v>
+        <v>4.6520000000000001</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -28493,7 +28592,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J42">
-        <v>5.2290000000000001</v>
+        <v>3.71</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -28528,7 +28627,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J43">
-        <v>5.4210000000000003</v>
+        <v>3.5750000000000002</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -28563,7 +28662,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J44">
-        <v>5.5439999999999996</v>
+        <v>3.8380000000000001</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -28598,7 +28697,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J45">
-        <v>5.6429999999999998</v>
+        <v>3.996</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -28633,7 +28732,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J46">
-        <v>5.8319999999999999</v>
+        <v>3.8820000000000001</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -28668,7 +28767,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J47">
-        <v>5.2389999999999999</v>
+        <v>3.64</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -28703,7 +28802,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J48">
-        <v>5.2949999999999999</v>
+        <v>3.6960000000000002</v>
       </c>
       <c r="K48">
         <v>1</v>
@@ -28738,7 +28837,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J49">
-        <v>5.0140000000000002</v>
+        <v>3.7360000000000002</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -28773,7 +28872,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J50">
-        <v>5.3369999999999997</v>
+        <v>3.6269999999999998</v>
       </c>
       <c r="K50">
         <v>1</v>
@@ -28808,7 +28907,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J51">
-        <v>5.5039999999999996</v>
+        <v>3.6880000000000002</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -28843,7 +28942,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J52">
-        <v>5.234</v>
+        <v>3.613</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -28878,7 +28977,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J53">
-        <v>5.5640000000000001</v>
+        <v>4.1459999999999999</v>
       </c>
       <c r="K53">
         <v>1</v>
@@ -28913,7 +29012,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J54">
-        <v>5.4580000000000002</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -28948,7 +29047,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J55">
-        <v>5.444</v>
+        <v>3.375</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -28983,7 +29082,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J56">
-        <v>5.2430000000000003</v>
+        <v>3.7669999999999999</v>
       </c>
       <c r="K56">
         <v>1</v>
@@ -29018,7 +29117,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J57">
-        <v>5.3639999999999999</v>
+        <v>3.7570000000000001</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -29053,7 +29152,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J58">
-        <v>5.3810000000000002</v>
+        <v>3.2839999999999998</v>
       </c>
       <c r="K58">
         <v>1</v>
@@ -29088,7 +29187,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J59">
-        <v>5.5369999999999999</v>
+        <v>3.867</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -29123,7 +29222,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J60">
-        <v>5.0190000000000001</v>
+        <v>3.6080000000000001</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -29158,7 +29257,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J61">
-        <v>5.1360000000000001</v>
+        <v>4.125</v>
       </c>
       <c r="K61">
         <v>1</v>
@@ -29193,7 +29292,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J62">
-        <v>5.19</v>
+        <v>3.7789999999999999</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -29228,7 +29327,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J63">
-        <v>5.298</v>
+        <v>4.0540000000000003</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -29263,7 +29362,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J64">
-        <v>5.8259999999999996</v>
+        <v>3.4820000000000002</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -29298,7 +29397,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J65">
-        <v>5.92</v>
+        <v>3.379</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -29333,7 +29432,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J66">
-        <v>5.3470000000000004</v>
+        <v>4.6360000000000001</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -29368,7 +29467,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J67">
-        <v>5.1719999999999997</v>
+        <v>3.9350000000000001</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -29403,7 +29502,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J68">
-        <v>5.1390000000000002</v>
+        <v>4.1840000000000002</v>
       </c>
       <c r="K68">
         <v>1</v>
@@ -29438,7 +29537,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J69">
-        <v>5.1459999999999999</v>
+        <v>3.8140000000000001</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -29473,7 +29572,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J70">
-        <v>5.6029999999999998</v>
+        <v>4.1420000000000003</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -29508,7 +29607,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J71">
-        <v>5.4539999999999997</v>
+        <v>4.2060000000000004</v>
       </c>
       <c r="K71">
         <v>1</v>
@@ -29543,7 +29642,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J72">
-        <v>5.1820000000000004</v>
+        <v>4.157</v>
       </c>
       <c r="K72">
         <v>1</v>
@@ -29578,7 +29677,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J73">
-        <v>5.8250000000000002</v>
+        <v>4.6539999999999999</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -29613,7 +29712,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J74">
-        <v>5.0739999999999998</v>
+        <v>4.319</v>
       </c>
       <c r="K74">
         <v>1</v>
@@ -29648,7 +29747,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J75">
-        <v>5.0430000000000001</v>
+        <v>4.6219999999999999</v>
       </c>
       <c r="K75">
         <v>1</v>
@@ -29683,7 +29782,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J76">
-        <v>4.8890000000000002</v>
+        <v>4.41</v>
       </c>
       <c r="K76">
         <v>1</v>
@@ -29718,7 +29817,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J77">
-        <v>5.6420000000000003</v>
+        <v>4.3529999999999998</v>
       </c>
       <c r="K77">
         <v>1</v>
@@ -29753,7 +29852,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J78">
-        <v>5.2220000000000004</v>
+        <v>4.0720000000000001</v>
       </c>
       <c r="K78">
         <v>1</v>
@@ -29788,7 +29887,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J79">
-        <v>5.2350000000000003</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K79">
         <v>1</v>
@@ -29823,7 +29922,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J80">
-        <v>5.2329999999999997</v>
+        <v>4.1289999999999996</v>
       </c>
       <c r="K80">
         <v>1</v>
@@ -29858,7 +29957,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J81">
-        <v>4.835</v>
+        <v>4.5010000000000003</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -29893,7 +29992,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J82">
-        <v>5.5049999999999999</v>
+        <v>3.9209999999999998</v>
       </c>
       <c r="K82">
         <v>1</v>
@@ -29928,7 +30027,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J83">
-        <v>5.2830000000000004</v>
+        <v>4.03</v>
       </c>
       <c r="K83">
         <v>1</v>
@@ -29963,7 +30062,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J84">
-        <v>4.7699999999999996</v>
+        <v>4.05</v>
       </c>
       <c r="K84">
         <v>1</v>
@@ -29998,7 +30097,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J85">
-        <v>5.3440000000000003</v>
+        <v>4.0780000000000003</v>
       </c>
       <c r="K85">
         <v>1</v>
@@ -30033,7 +30132,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J86">
-        <v>5.0919999999999996</v>
+        <v>4.5739999999999998</v>
       </c>
       <c r="K86">
         <v>1</v>
@@ -30068,7 +30167,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J87">
-        <v>5.1740000000000004</v>
+        <v>4.3659999999999997</v>
       </c>
       <c r="K87">
         <v>1</v>
@@ -30103,7 +30202,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J88">
-        <v>5.0259999999999998</v>
+        <v>4.78</v>
       </c>
       <c r="K88">
         <v>1</v>
@@ -30138,7 +30237,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J89">
-        <v>5.0780000000000003</v>
+        <v>4.2869999999999999</v>
       </c>
       <c r="K89">
         <v>1</v>
@@ -30173,7 +30272,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J90">
-        <v>5.2969999999999997</v>
+        <v>4.133</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -30208,7 +30307,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J91">
-        <v>5.1340000000000003</v>
+        <v>4.3090000000000002</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -30243,7 +30342,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J92">
-        <v>4.9290000000000003</v>
+        <v>4.0860000000000003</v>
       </c>
       <c r="K92">
         <v>1</v>
@@ -30278,7 +30377,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J93">
-        <v>5.5439999999999996</v>
+        <v>4.0819999999999999</v>
       </c>
       <c r="K93">
         <v>1</v>
@@ -30313,7 +30412,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J94">
-        <v>5.39</v>
+        <v>4.1050000000000004</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -30348,7 +30447,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J95">
-        <v>5.22</v>
+        <v>4.3819999999999997</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -30383,7 +30482,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J96">
-        <v>4.8840000000000003</v>
+        <v>4.5750000000000002</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -30418,7 +30517,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J97">
-        <v>5.6109999999999998</v>
+        <v>4.3979999999999997</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -30453,7 +30552,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J98">
-        <v>5.1379999999999999</v>
+        <v>4.0910000000000002</v>
       </c>
       <c r="K98">
         <v>1</v>
@@ -30488,7 +30587,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J99">
-        <v>5.7039999999999997</v>
+        <v>4.4610000000000003</v>
       </c>
       <c r="K99">
         <v>1</v>
@@ -30523,7 +30622,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J100">
-        <v>5.1369999999999996</v>
+        <v>4.1829999999999998</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -30558,7 +30657,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J101">
-        <v>5.5259999999999998</v>
+        <v>4.141</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -30593,7 +30692,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J102">
-        <v>5.3360000000000003</v>
+        <v>4.1390000000000002</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -30628,7 +30727,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J103">
-        <v>5.2960000000000003</v>
+        <v>3.9740000000000002</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -30663,7 +30762,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J104">
-        <v>5.1390000000000002</v>
+        <v>3.9329999999999998</v>
       </c>
       <c r="K104">
         <v>1</v>
@@ -30698,7 +30797,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J105">
-        <v>4.95</v>
+        <v>4.4180000000000001</v>
       </c>
       <c r="K105">
         <v>1</v>
@@ -30733,7 +30832,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J106">
-        <v>5.1079999999999997</v>
+        <v>4.7169999999999996</v>
       </c>
       <c r="K106">
         <v>1</v>
@@ -30768,7 +30867,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J107">
-        <v>5.1760000000000002</v>
+        <v>4.5990000000000002</v>
       </c>
       <c r="K107">
         <v>1</v>
@@ -30803,7 +30902,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J108">
-        <v>5.1459999999999999</v>
+        <v>4.3330000000000002</v>
       </c>
       <c r="K108">
         <v>1</v>
@@ -30838,7 +30937,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J109">
-        <v>5.2220000000000004</v>
+        <v>4.718</v>
       </c>
       <c r="K109">
         <v>1</v>
@@ -30873,7 +30972,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J110">
-        <v>5.5739999999999998</v>
+        <v>4.6109999999999998</v>
       </c>
       <c r="K110">
         <v>1</v>
@@ -30908,7 +31007,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J111">
-        <v>5.0289999999999999</v>
+        <v>4.2939999999999996</v>
       </c>
       <c r="K111">
         <v>1</v>
@@ -30943,7 +31042,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J112">
-        <v>4.9740000000000002</v>
+        <v>4.1180000000000003</v>
       </c>
       <c r="K112">
         <v>1</v>
@@ -30978,7 +31077,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J113">
-        <v>4.7649999999999997</v>
+        <v>3.9929999999999999</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -31013,7 +31112,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J114">
-        <v>4.8920000000000003</v>
+        <v>4.0860000000000003</v>
       </c>
       <c r="K114">
         <v>1</v>
@@ -31048,7 +31147,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J115">
-        <v>4.9420000000000002</v>
+        <v>3.847</v>
       </c>
       <c r="K115">
         <v>1</v>
@@ -31083,7 +31182,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J116">
-        <v>5.0659999999999998</v>
+        <v>3.851</v>
       </c>
       <c r="K116">
         <v>1</v>
@@ -31118,7 +31217,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J117">
-        <v>5.3550000000000004</v>
+        <v>4.1479999999999997</v>
       </c>
       <c r="K117">
         <v>1</v>
@@ -31153,7 +31252,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J118">
-        <v>4.9560000000000004</v>
+        <v>4.4059999999999997</v>
       </c>
       <c r="K118">
         <v>1</v>
@@ -31188,7 +31287,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J119">
-        <v>5.0679999999999996</v>
+        <v>3.879</v>
       </c>
       <c r="K119">
         <v>1</v>
@@ -31223,7 +31322,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J120">
-        <v>4.9180000000000001</v>
+        <v>4.0519999999999996</v>
       </c>
       <c r="K120">
         <v>1</v>
@@ -31258,7 +31357,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J121">
-        <v>5.4269999999999996</v>
+        <v>4.1550000000000002</v>
       </c>
       <c r="K121">
         <v>1</v>
@@ -31293,7 +31392,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J122">
-        <v>4.8479999999999999</v>
+        <v>4.2850000000000001</v>
       </c>
       <c r="K122">
         <v>1</v>
@@ -31328,7 +31427,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J123">
-        <v>5.5229999999999997</v>
+        <v>4.0620000000000003</v>
       </c>
       <c r="K123">
         <v>1</v>
@@ -31363,7 +31462,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J124">
-        <v>5.367</v>
+        <v>4.2460000000000004</v>
       </c>
       <c r="K124">
         <v>1</v>
@@ -31398,7 +31497,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J125">
-        <v>5.0739999999999998</v>
+        <v>4.8230000000000004</v>
       </c>
       <c r="K125">
         <v>1</v>
@@ -31433,7 +31532,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J126">
-        <v>5.1459999999999999</v>
+        <v>4.5960000000000001</v>
       </c>
       <c r="K126">
         <v>1</v>
@@ -31468,7 +31567,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J127">
-        <v>5.0739999999999998</v>
+        <v>4.4550000000000001</v>
       </c>
       <c r="K127">
         <v>1</v>
@@ -31503,7 +31602,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J128">
-        <v>4.8319999999999999</v>
+        <v>4.2190000000000003</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -31538,7 +31637,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J129">
-        <v>5.1429999999999998</v>
+        <v>4.3529999999999998</v>
       </c>
       <c r="K129">
         <v>1</v>
@@ -31573,7 +31672,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J130">
-        <v>4.9130000000000003</v>
+        <v>4.282</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -31608,7 +31707,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J131">
-        <v>4.8570000000000002</v>
+        <v>4.4820000000000002</v>
       </c>
       <c r="K131">
         <v>1</v>
@@ -31643,7 +31742,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J132">
-        <v>5.1150000000000002</v>
+        <v>3.8740000000000001</v>
       </c>
       <c r="K132">
         <v>1</v>
@@ -31678,7 +31777,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J133">
-        <v>5.3339999999999996</v>
+        <v>4.2590000000000003</v>
       </c>
       <c r="K133">
         <v>1</v>
@@ -31713,7 +31812,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J134">
-        <v>5.069</v>
+        <v>4.51</v>
       </c>
       <c r="K134">
         <v>1</v>
@@ -31748,7 +31847,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J135">
-        <v>5.2430000000000003</v>
+        <v>4.7329999999999997</v>
       </c>
       <c r="K135">
         <v>1</v>
@@ -31783,7 +31882,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J136">
-        <v>4.9889999999999999</v>
+        <v>4.3540000000000001</v>
       </c>
       <c r="K136">
         <v>1</v>
@@ -31818,7 +31917,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J137">
-        <v>4.976</v>
+        <v>4.0860000000000003</v>
       </c>
       <c r="K137">
         <v>1</v>
@@ -31853,7 +31952,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J138">
-        <v>4.9989999999999997</v>
+        <v>4.1139999999999999</v>
       </c>
       <c r="K138">
         <v>1</v>
@@ -31888,7 +31987,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J139">
-        <v>5.048</v>
+        <v>4.0460000000000003</v>
       </c>
       <c r="K139">
         <v>1</v>
@@ -31923,7 +32022,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J140">
-        <v>5.0629999999999997</v>
+        <v>3.9860000000000002</v>
       </c>
       <c r="K140">
         <v>1</v>
@@ -31958,7 +32057,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J141">
-        <v>5.6769999999999996</v>
+        <v>3.9249999999999998</v>
       </c>
       <c r="K141">
         <v>1</v>
@@ -31993,7 +32092,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J142">
-        <v>5.0650000000000004</v>
+        <v>4.1849999999999996</v>
       </c>
       <c r="K142">
         <v>1</v>
@@ -32028,7 +32127,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J143">
-        <v>5.4089999999999998</v>
+        <v>4.4809999999999999</v>
       </c>
       <c r="K143">
         <v>1</v>
@@ -32063,7 +32162,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J144">
-        <v>5.2720000000000002</v>
+        <v>4.3940000000000001</v>
       </c>
       <c r="K144">
         <v>1</v>
@@ -32098,7 +32197,7 @@
         <v>0.99865000000000004</v>
       </c>
       <c r="J145">
-        <v>5.7279999999999998</v>
+        <v>4.6269999999999998</v>
       </c>
       <c r="K145">
         <v>1</v>
@@ -32133,7 +32232,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J146">
-        <v>5.0430000000000001</v>
+        <v>4.3170000000000002</v>
       </c>
       <c r="K146">
         <v>1</v>
@@ -32168,7 +32267,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J147">
-        <v>4.8470000000000004</v>
+        <v>4.375</v>
       </c>
       <c r="K147">
         <v>1</v>
@@ -32203,7 +32302,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J148">
-        <v>4.891</v>
+        <v>4.1719999999999997</v>
       </c>
       <c r="K148">
         <v>1</v>
@@ -32238,7 +32337,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J149">
-        <v>5.0250000000000004</v>
+        <v>4.101</v>
       </c>
       <c r="K149">
         <v>1</v>
@@ -32273,7 +32372,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J150">
-        <v>5.1219999999999999</v>
+        <v>4.0149999999999997</v>
       </c>
       <c r="K150">
         <v>1</v>
@@ -32308,7 +32407,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J151">
-        <v>5.444</v>
+        <v>3.86</v>
       </c>
       <c r="K151">
         <v>1</v>
@@ -32343,7 +32442,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J152">
-        <v>5.1719999999999997</v>
+        <v>4.1989999999999998</v>
       </c>
       <c r="K152">
         <v>1</v>
@@ -32378,7 +32477,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J153">
-        <v>4.9509999999999996</v>
+        <v>4.181</v>
       </c>
       <c r="K153">
         <v>1</v>
@@ -32413,7 +32512,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J154">
-        <v>5.266</v>
+        <v>4.03</v>
       </c>
       <c r="K154">
         <v>1</v>
@@ -32448,7 +32547,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J155">
-        <v>5.008</v>
+        <v>3.9740000000000002</v>
       </c>
       <c r="K155">
         <v>1</v>
@@ -32483,7 +32582,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J156">
-        <v>5.3879999999999999</v>
+        <v>4.1740000000000004</v>
       </c>
       <c r="K156">
         <v>1</v>
@@ -32518,7 +32617,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J157">
-        <v>5.2939999999999996</v>
+        <v>4.2549999999999999</v>
       </c>
       <c r="K157">
         <v>1</v>
@@ -32553,7 +32652,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J158">
-        <v>5.6959999999999997</v>
+        <v>4.1779999999999999</v>
       </c>
       <c r="K158">
         <v>1</v>
@@ -32588,7 +32687,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J159">
-        <v>4.8540000000000001</v>
+        <v>3.9009999999999998</v>
       </c>
       <c r="K159">
         <v>1</v>
@@ -32623,7 +32722,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J160">
-        <v>5.444</v>
+        <v>4.5910000000000002</v>
       </c>
       <c r="K160">
         <v>1</v>
@@ -32658,7 +32757,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J161">
-        <v>5.5439999999999996</v>
+        <v>4.1239999999999997</v>
       </c>
       <c r="K161">
         <v>1</v>
@@ -32693,7 +32792,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J162">
-        <v>5.1449999999999996</v>
+        <v>4.6840000000000002</v>
       </c>
       <c r="K162">
         <v>1</v>
@@ -32728,7 +32827,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J163">
-        <v>5.3940000000000001</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="K163">
         <v>1</v>
@@ -32763,7 +32862,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J164">
-        <v>5.0380000000000003</v>
+        <v>4.1289999999999996</v>
       </c>
       <c r="K164">
         <v>1</v>
@@ -32798,7 +32897,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J165">
-        <v>4.9160000000000004</v>
+        <v>4.149</v>
       </c>
       <c r="K165">
         <v>1</v>
@@ -32833,7 +32932,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J166">
-        <v>5.16</v>
+        <v>4.0289999999999999</v>
       </c>
       <c r="K166">
         <v>1</v>
@@ -32868,7 +32967,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J167">
-        <v>5.0110000000000001</v>
+        <v>4.0819999999999999</v>
       </c>
       <c r="K167">
         <v>1</v>
@@ -32903,7 +33002,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J168">
-        <v>5.5010000000000003</v>
+        <v>4.0739999999999998</v>
       </c>
       <c r="K168">
         <v>1</v>
@@ -32938,7 +33037,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J169">
-        <v>5.0579999999999998</v>
+        <v>3.8620000000000001</v>
       </c>
       <c r="K169">
         <v>1</v>
@@ -32973,7 +33072,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J170">
-        <v>5.3970000000000002</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="K170">
         <v>1</v>
@@ -33008,7 +33107,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J171">
-        <v>5.1340000000000003</v>
+        <v>4.3890000000000002</v>
       </c>
       <c r="K171">
         <v>1</v>
@@ -33043,7 +33142,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J172">
-        <v>5.351</v>
+        <v>4.0970000000000004</v>
       </c>
       <c r="K172">
         <v>1</v>
@@ -33078,7 +33177,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J173">
-        <v>4.9790000000000001</v>
+        <v>4.07</v>
       </c>
       <c r="K173">
         <v>1</v>
@@ -33113,7 +33212,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J174">
-        <v>5.43</v>
+        <v>3.67</v>
       </c>
       <c r="K174">
         <v>1</v>
@@ -33148,7 +33247,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J175">
-        <v>5.0919999999999996</v>
+        <v>4.21</v>
       </c>
       <c r="K175">
         <v>1</v>
@@ -33183,7 +33282,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J176">
-        <v>5.2949999999999999</v>
+        <v>4.1020000000000003</v>
       </c>
       <c r="K176">
         <v>1</v>
@@ -33218,7 +33317,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J177">
-        <v>5.3879999999999999</v>
+        <v>4.6210000000000004</v>
       </c>
       <c r="K177">
         <v>1</v>
@@ -33253,7 +33352,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J178">
-        <v>5.5759999999999996</v>
+        <v>3.9910000000000001</v>
       </c>
       <c r="K178">
         <v>1</v>
@@ -33288,7 +33387,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J179">
-        <v>5.2919999999999998</v>
+        <v>5.1959999999999997</v>
       </c>
       <c r="K179">
         <v>1</v>
@@ -33323,7 +33422,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J180">
-        <v>5.4119999999999999</v>
+        <v>4.8780000000000001</v>
       </c>
       <c r="K180">
         <v>1</v>
@@ -33358,7 +33457,7 @@
         <v>0.99819999999999998</v>
       </c>
       <c r="J181">
-        <v>5.4260000000000002</v>
+        <v>4.1269999999999998</v>
       </c>
       <c r="K181">
         <v>1</v>

</xml_diff>